<commit_message>
Added interesting graph in excel doc
</commit_message>
<xml_diff>
--- a/spec/prototype_large_project.xlsx
+++ b/spec/prototype_large_project.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19725" windowHeight="9135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19725" windowHeight="9135" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -1458,11 +1459,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="499449880"/>
-        <c:axId val="499442432"/>
+        <c:axId val="399547952"/>
+        <c:axId val="399546384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="499449880"/>
+        <c:axId val="399547952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1519,12 +1520,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="499442432"/>
+        <c:crossAx val="399546384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="499442432"/>
+        <c:axId val="399546384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1581,7 +1582,988 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="499449880"/>
+        <c:crossAx val="399547952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sv-SE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Second part is power distributed</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sv-SE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="sv-SE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$1:$A$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="104"/>
+                <c:pt idx="71">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>293</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>349</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>371</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>374</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>449</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>467</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>483</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>491</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>559</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>583</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>599</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>636</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>687</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>708</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>841</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="424348848"/>
+        <c:axId val="424351200"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="424348848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="424351200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="424351200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="424348848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="sv-SE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>First part is linear</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="sv-SE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="sv-SE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$B$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="106"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>193</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="424347672"/>
+        <c:axId val="424345712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="424347672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="424345712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="424345712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sv-SE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="424347672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1670,7 +2652,1123 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2215,6 +4313,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>595312</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>109537</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>414337</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2488,8 +4651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4584,4 +6747,640 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B105"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>241</v>
+      </c>
+      <c r="B78" s="2"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>244</v>
+      </c>
+      <c r="B79" s="2"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>247</v>
+      </c>
+      <c r="B80" s="2"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>258</v>
+      </c>
+      <c r="B81" s="2"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>260</v>
+      </c>
+      <c r="B82" s="2"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>268</v>
+      </c>
+      <c r="B83" s="2"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>270</v>
+      </c>
+      <c r="B84" s="2"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>293</v>
+      </c>
+      <c r="B85" s="2"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>320</v>
+      </c>
+      <c r="B86" s="2"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>349</v>
+      </c>
+      <c r="B87" s="2"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>371</v>
+      </c>
+      <c r="B88" s="2"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>374</v>
+      </c>
+      <c r="B89" s="2"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>416</v>
+      </c>
+      <c r="B90" s="2"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>449</v>
+      </c>
+      <c r="B91" s="2"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>467</v>
+      </c>
+      <c r="B92" s="2"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>483</v>
+      </c>
+      <c r="B93" s="2"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>491</v>
+      </c>
+      <c r="B94" s="2"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>525</v>
+      </c>
+      <c r="B95" s="2"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>559</v>
+      </c>
+      <c r="B96" s="2"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>583</v>
+      </c>
+      <c r="B97" s="2"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>599</v>
+      </c>
+      <c r="B98" s="2"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>636</v>
+      </c>
+      <c r="B99" s="2"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>687</v>
+      </c>
+      <c r="B100" s="2"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>708</v>
+      </c>
+      <c r="B101" s="2"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>841</v>
+      </c>
+      <c r="B102" s="2"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>1125</v>
+      </c>
+      <c r="B103" s="2"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B104" s="2"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B105" s="2"/>
+    </row>
+  </sheetData>
+  <sortState ref="B1:B104">
+    <sortCondition ref="B1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Showing regression linear function in diagram
</commit_message>
<xml_diff>
--- a/spec/prototype_large_project.xlsx
+++ b/spec/prototype_large_project.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19725" windowHeight="9135" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24525" windowHeight="13635"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -780,7 +780,7 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1459,11 +1459,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="399547952"/>
-        <c:axId val="399546384"/>
+        <c:axId val="407115824"/>
+        <c:axId val="407114648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="399547952"/>
+        <c:axId val="407115824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1520,12 +1520,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399546384"/>
+        <c:crossAx val="407114648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="399546384"/>
+        <c:axId val="407114648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1582,7 +1582,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399547952"/>
+        <c:crossAx val="407115824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1892,11 +1892,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="424348848"/>
-        <c:axId val="424351200"/>
+        <c:axId val="407117392"/>
+        <c:axId val="407116216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="424348848"/>
+        <c:axId val="407117392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1952,12 +1952,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424351200"/>
+        <c:crossAx val="407116216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="424351200"/>
+        <c:axId val="407116216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2014,7 +2014,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424348848"/>
+        <c:crossAx val="407117392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2441,11 +2441,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="424347672"/>
-        <c:axId val="424345712"/>
+        <c:axId val="407111904"/>
+        <c:axId val="407112296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="424347672"/>
+        <c:axId val="407111904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2501,12 +2501,12 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424345712"/>
+        <c:crossAx val="407112296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="424345712"/>
+        <c:axId val="407112296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2563,7 +2563,7 @@
             <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424347672"/>
+        <c:crossAx val="407111904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4651,7 +4651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -6753,7 +6753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>